<commit_message>
Added Log4j and ExtentReport
</commit_message>
<xml_diff>
--- a/AdactinAutomation/src/test/resources/TestData/Testdata.xlsx
+++ b/AdactinAutomation/src/test/resources/TestData/Testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\eclipse\selenium workspace\AdactinAutomation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\repository-adactin\AdactinAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DA59AA-8FF4-46D6-BB0B-282737758C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1675E8-3285-4790-9AB3-F3ED9E7B32D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FAC7BE58-BA04-42C1-B782-02BD2684E890}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FAC7BE58-BA04-42C1-B782-02BD2684E890}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,6 +203,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,16 +520,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A6A35B-34B2-4273-9A2C-687BE4A1DFC6}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -546,19 +549,31 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -570,17 +585,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B204616F-2F7F-494E-B577-6378A0555D54}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -602,10 +620,10 @@
       <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -643,69 +661,121 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F638864-6638-44B7-9B2E-4612903006F6}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" customWidth="1"/>
-    <col min="6" max="7" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" customWidth="1"/>
+    <col min="12" max="12" width="19.90625" customWidth="1"/>
+    <col min="13" max="13" width="18.90625" customWidth="1"/>
+    <col min="14" max="15" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8">
+        <v>45806</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45807</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>